<commit_message>
Added Links to Schedule
</commit_message>
<xml_diff>
--- a/BCB520/posts/Syllabus/Schedule.xlsx
+++ b/BCB520/posts/Syllabus/Schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/barrierobison/Documents/GitHub/RobisonWeb/BCB520/posts/Syllabus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C035FFA-B073-EC47-9CA0-4FDC250FD8E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C2EE179-A501-B94C-B945-893F67A9D831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{EBCA7641-3948-9148-9861-B8FB99728971}"/>
+    <workbookView xWindow="1060" yWindow="1740" windowWidth="30940" windowHeight="17880" xr2:uid="{EBCA7641-3948-9148-9861-B8FB99728971}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -47,15 +47,9 @@
     <t>READING</t>
   </si>
   <si>
-    <t>INTRODUCTION.  Why Visualization Matters</t>
-  </si>
-  <si>
     <t>VAD Ch 1.</t>
   </si>
   <si>
-    <t>Assignment 1 - Fun with literate programming.</t>
-  </si>
-  <si>
     <t>WHAT?  Abstraction of Data</t>
   </si>
   <si>
@@ -225,13 +219,19 @@
   </si>
   <si>
     <t>Portfolio Review</t>
+  </si>
+  <si>
+    <t>[Assignment 1](/BCB520/posts/A1-Lit-Prog) - Fun with literate programming.</t>
+  </si>
+  <si>
+    <t>[INTRODUCTION](/BCB520/posts/L1-Intro).  Why Visualization Matters</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -252,14 +252,6 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -278,19 +270,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="15" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -409,7 +400,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -697,7 +688,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -708,7 +699,7 @@
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -732,24 +723,24 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>44938</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>4</v>
-      </c>
       <c r="D2" s="4" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="E2" s="3"/>
     </row>
@@ -758,14 +749,14 @@
         <v>44943</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="4" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="20" x14ac:dyDescent="0.2">
@@ -773,13 +764,13 @@
         <v>44945</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E4" s="3"/>
     </row>
@@ -788,10 +779,10 @@
         <v>44950</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
@@ -801,13 +792,13 @@
         <v>44952</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E6" s="3"/>
     </row>
@@ -816,10 +807,10 @@
         <v>44957</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
@@ -829,13 +820,13 @@
         <v>44959</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E8" s="3"/>
     </row>
@@ -844,10 +835,10 @@
         <v>44964</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -857,13 +848,13 @@
         <v>44966</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E10" s="3"/>
     </row>
@@ -872,10 +863,10 @@
         <v>44971</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -885,12 +876,12 @@
         <v>44973</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="20" x14ac:dyDescent="0.2">
@@ -898,12 +889,12 @@
         <v>44978</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="20" x14ac:dyDescent="0.2">
@@ -911,13 +902,13 @@
         <v>44980</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E14" s="3"/>
     </row>
@@ -926,10 +917,10 @@
         <v>44985</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -939,13 +930,13 @@
         <v>44987</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E16" s="3"/>
     </row>
@@ -954,10 +945,10 @@
         <v>44992</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
@@ -967,13 +958,13 @@
         <v>44994</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E18" s="3"/>
     </row>
@@ -982,12 +973,12 @@
         <v>44999</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="20" x14ac:dyDescent="0.2">
@@ -995,12 +986,12 @@
         <v>45001</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="20" x14ac:dyDescent="0.2">
@@ -1008,10 +999,10 @@
         <v>45006</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
@@ -1021,13 +1012,13 @@
         <v>45008</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E22" s="3"/>
     </row>
@@ -1036,10 +1027,10 @@
         <v>45013</v>
       </c>
       <c r="B23" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="E23" s="3"/>
     </row>
@@ -1048,13 +1039,13 @@
         <v>45015</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E24" s="3"/>
     </row>
@@ -1063,10 +1054,10 @@
         <v>45020</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
@@ -1076,13 +1067,13 @@
         <v>45022</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E26" s="3"/>
     </row>
@@ -1091,10 +1082,10 @@
         <v>45027</v>
       </c>
       <c r="B27" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
@@ -1104,12 +1095,12 @@
         <v>45029</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="20" x14ac:dyDescent="0.2">
@@ -1117,7 +1108,7 @@
         <v>45034</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
@@ -1128,7 +1119,7 @@
         <v>45036</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
@@ -1139,12 +1130,12 @@
         <v>45041</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="20" x14ac:dyDescent="0.2">
@@ -1152,12 +1143,12 @@
         <v>45043</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="20" x14ac:dyDescent="0.2">
@@ -1165,11 +1156,11 @@
         <v>45048</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E33" s="3"/>
     </row>
@@ -1178,11 +1169,11 @@
         <v>45050</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E34" s="3"/>
     </row>
@@ -1191,16 +1182,12 @@
         <v>45055</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C35" s="3"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" tooltip="Assignment 1 - Fun with literate programming." display="https://canvas.uidaho.edu/courses/17806/assignments/188565" xr:uid="{D0B587EE-DA5B-1545-824D-FA94AA457381}"/>
-    <hyperlink ref="E3" r:id="rId2" tooltip="Assignment 1 - Fun with literate programming." display="https://canvas.uidaho.edu/courses/17806/assignments/188565" xr:uid="{28661C6A-081D-C54E-8917-75E58319BE81}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>